<commit_message>
Added option to select video from dropdown menu
</commit_message>
<xml_diff>
--- a/Keyword Extraction/Results_Detailed Accuracy/detailedAccuracy_Video_3_BodyProject.txt.xlsx
+++ b/Keyword Extraction/Results_Detailed Accuracy/detailedAccuracy_Video_3_BodyProject.txt.xlsx
@@ -1375,10 +1375,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>81.34942054748535</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1400,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>97.16835021972656</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1430,10 +1430,10 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>99.99997615814209</v>
+        <v>64.26011323928833</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1444,7 +1444,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>99.9998927116394</v>
+        <v>99.10577535629272</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1452,10 +1452,10 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>99.99967813491821</v>
+        <v>99.9972939491272</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1499,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>99.96368885040283</v>
+        <v>99.75234866142273</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1510,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>99.52530860900879</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1521,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>97.71247506141663</v>
+        <v>99.86864924430847</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1532,7 +1532,7 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1543,7 +1543,7 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>99.94685053825378</v>
+        <v>91.86967611312866</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1554,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1587,7 +1587,7 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>99.99998807907104</v>
+        <v>98.4327495098114</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>99.99994039535522</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1609,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>100</v>
+        <v>99.99978542327881</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1620,7 +1620,7 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1628,10 +1628,10 @@
         <v>26</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>99.97918009757996</v>
+        <v>93.96571516990662</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1642,7 +1642,7 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>99.99541044235229</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1650,10 +1650,10 @@
         <v>28</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>99.99998807907104</v>
+        <v>99.99473094940186</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1664,7 +1664,7 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>99.99990463256836</v>
+        <v>99.99133348464966</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1675,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>99.99995231628418</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1686,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>99.99985694885254</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1697,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1708,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>100</v>
+        <v>99.98739957809448</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1719,7 +1719,7 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <v>99.99899864196777</v>
+        <v>99.99898672103882</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1730,7 +1730,7 @@
         <v>2</v>
       </c>
       <c r="D34">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1763,7 +1763,7 @@
         <v>2</v>
       </c>
       <c r="D37">
-        <v>100</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1785,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1793,10 +1793,10 @@
         <v>41</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>99.99991655349731</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1818,7 +1818,7 @@
         <v>2</v>
       </c>
       <c r="D42">
-        <v>99.99984502792358</v>
+        <v>99.99980926513672</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1829,7 +1829,7 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <v>99.9998927116394</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1840,7 +1840,7 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <v>99.99179840087891</v>
+        <v>99.67779517173767</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1851,7 +1851,7 @@
         <v>2</v>
       </c>
       <c r="D45">
-        <v>100</v>
+        <v>99.99951124191284</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1862,7 +1862,7 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1873,7 +1873,7 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <v>99.9997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1884,7 +1884,7 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <v>99.99996423721313</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1892,10 +1892,10 @@
         <v>50</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>99.9983549118042</v>
+        <v>66.74056053161621</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1906,7 +1906,7 @@
         <v>2</v>
       </c>
       <c r="D50">
-        <v>99.99436140060425</v>
+        <v>99.99922513961792</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1917,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="D51">
-        <v>99.99996423721313</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1939,7 +1939,7 @@
         <v>2</v>
       </c>
       <c r="D53">
-        <v>100</v>
+        <v>99.99972581863403</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1961,7 +1961,7 @@
         <v>2</v>
       </c>
       <c r="D55">
-        <v>99.99996423721313</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1969,10 +1969,10 @@
         <v>57</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56">
-        <v>100</v>
+        <v>99.79694485664368</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1983,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="D57">
-        <v>99.99990463256836</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <v>99.99998807907104</v>
+        <v>99.99781847000122</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2016,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="D60">
-        <v>99.99579191207886</v>
+        <v>99.99973773956299</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2027,7 +2027,7 @@
         <v>2</v>
       </c>
       <c r="D61">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2038,7 +2038,7 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>99.92257356643677</v>
+        <v>99.48304295539856</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2049,7 +2049,7 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>99.9998927116394</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2060,7 +2060,7 @@
         <v>2</v>
       </c>
       <c r="D64">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2093,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="D67">
-        <v>98.33196997642517</v>
+        <v>77.62854695320129</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2104,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2112,10 +2112,10 @@
         <v>70</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>99.9757707118988</v>
+        <v>89.67294692993164</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2148,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="D72">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2159,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>99.99997615814209</v>
+        <v>93.74159574508667</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2170,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="D74">
-        <v>99.99978542327881</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2181,7 +2181,7 @@
         <v>2</v>
       </c>
       <c r="D75">
-        <v>94.11141872406006</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2192,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="D76">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2203,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="D77">
-        <v>98.95434379577637</v>
+        <v>99.97516274452209</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2214,7 +2214,7 @@
         <v>2</v>
       </c>
       <c r="D78">
-        <v>99.99995231628418</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <v>99.99575614929199</v>
+        <v>99.81174468994141</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2236,7 +2236,7 @@
         <v>2</v>
       </c>
       <c r="D80">
-        <v>100</v>
+        <v>99.99972581863403</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2247,7 +2247,7 @@
         <v>2</v>
       </c>
       <c r="D81">
-        <v>99.99979734420776</v>
+        <v>99.99970197677612</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2258,7 +2258,7 @@
         <v>2</v>
       </c>
       <c r="D82">
-        <v>99.99899864196777</v>
+        <v>61.56633496284485</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2269,7 +2269,7 @@
         <v>2</v>
       </c>
       <c r="D83">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2277,10 +2277,10 @@
         <v>85</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D84">
-        <v>100</v>
+        <v>88.8554573059082</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2291,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="D85">
-        <v>99.9998927116394</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2313,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="D87">
-        <v>99.99990463256836</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2324,7 +2324,7 @@
         <v>1</v>
       </c>
       <c r="D88">
-        <v>99.99847412109375</v>
+        <v>99.99939203262329</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2332,10 +2332,10 @@
         <v>89</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89">
-        <v>99.80022311210632</v>
+        <v>99.59648847579956</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2343,10 +2343,10 @@
         <v>90</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90">
-        <v>99.50533509254456</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2354,10 +2354,10 @@
         <v>91</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D91">
-        <v>50.52620768547058</v>
+        <v>99.99979734420776</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2365,10 +2365,10 @@
         <v>92</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92">
-        <v>99.99983310699463</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2390,7 +2390,7 @@
         <v>2</v>
       </c>
       <c r="D94">
-        <v>99.99923706054688</v>
+        <v>99.98102784156799</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2401,7 +2401,7 @@
         <v>1</v>
       </c>
       <c r="D95">
-        <v>99.94757771492004</v>
+        <v>83.00496339797974</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2412,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="D96">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2423,7 +2423,7 @@
         <v>2</v>
       </c>
       <c r="D97">
-        <v>99.99988079071045</v>
+        <v>74.25695657730103</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2434,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="D98">
-        <v>99.99712705612183</v>
+        <v>98.52530360221863</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2445,7 +2445,7 @@
         <v>2</v>
       </c>
       <c r="D99">
-        <v>99.99992847442627</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2456,7 +2456,7 @@
         <v>2</v>
       </c>
       <c r="D100">
-        <v>99.99992847442627</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2522,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="D106">
-        <v>99.991774559021</v>
+        <v>99.9848484992981</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2533,7 +2533,7 @@
         <v>2</v>
       </c>
       <c r="D107">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2544,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="D108">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2555,7 +2555,7 @@
         <v>2</v>
       </c>
       <c r="D109">
-        <v>100</v>
+        <v>99.59557056427002</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2566,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="D110">
-        <v>78.88119220733643</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2577,7 +2577,7 @@
         <v>2</v>
       </c>
       <c r="D111">
-        <v>97.00239300727844</v>
+        <v>99.99992847442627</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2588,7 +2588,7 @@
         <v>2</v>
       </c>
       <c r="D112">
-        <v>99.99957084655762</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2599,7 +2599,7 @@
         <v>2</v>
       </c>
       <c r="D113">
-        <v>99.99282360076904</v>
+        <v>99.60421323776245</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2610,7 +2610,7 @@
         <v>2</v>
       </c>
       <c r="D114">
-        <v>100</v>
+        <v>99.99357461929321</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2632,7 +2632,7 @@
         <v>2</v>
       </c>
       <c r="D116">
-        <v>99.99954700469971</v>
+        <v>99.99992847442627</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2643,7 +2643,7 @@
         <v>1</v>
       </c>
       <c r="D117">
-        <v>97.34322428703308</v>
+        <v>94.60002183914185</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2651,10 +2651,10 @@
         <v>117</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D118">
-        <v>99.99990463256836</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2673,10 +2673,10 @@
         <v>119</v>
       </c>
       <c r="C120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D120">
-        <v>99.99977350234985</v>
+        <v>68.20457577705383</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2695,10 +2695,10 @@
         <v>121</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122">
-        <v>84.70350503921509</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2706,10 +2706,10 @@
         <v>122</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D123">
-        <v>99.99996423721313</v>
+        <v>77.8922975063324</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2720,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="D124">
-        <v>99.99996423721313</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2742,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="D126">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2753,7 +2753,7 @@
         <v>2</v>
       </c>
       <c r="D127">
-        <v>100</v>
+        <v>99.99940395355225</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2775,7 +2775,7 @@
         <v>2</v>
       </c>
       <c r="D129">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2797,7 +2797,7 @@
         <v>2</v>
       </c>
       <c r="D131">
-        <v>100</v>
+        <v>99.99973773956299</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2816,10 +2816,10 @@
         <v>132</v>
       </c>
       <c r="C133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D133">
-        <v>99.99992847442627</v>
+        <v>99.99144077301025</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2830,7 +2830,7 @@
         <v>2</v>
       </c>
       <c r="D134">
-        <v>99.99983310699463</v>
+        <v>99.99852180480957</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2841,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="D135">
-        <v>69.70750689506531</v>
+        <v>98.95802140235901</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2849,10 +2849,10 @@
         <v>135</v>
       </c>
       <c r="C136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D136">
-        <v>99.99998807907104</v>
+        <v>99.9796450138092</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2863,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="D137">
-        <v>99.93694424629211</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2885,7 +2885,7 @@
         <v>2</v>
       </c>
       <c r="D139">
-        <v>99.99996423721313</v>
+        <v>99.44407343864441</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2896,7 +2896,7 @@
         <v>1</v>
       </c>
       <c r="D140">
-        <v>99.88723397254944</v>
+        <v>80.96778988838196</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2904,10 +2904,10 @@
         <v>140</v>
       </c>
       <c r="C141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D141">
-        <v>99.99974966049194</v>
+        <v>96.88242077827454</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2915,10 +2915,10 @@
         <v>141</v>
       </c>
       <c r="C142">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D142">
-        <v>97.07183241844177</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2929,7 +2929,7 @@
         <v>2</v>
       </c>
       <c r="D143">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2951,7 +2951,7 @@
         <v>2</v>
       </c>
       <c r="D145">
-        <v>99.99995231628418</v>
+        <v>99.99321699142456</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2959,10 +2959,10 @@
         <v>145</v>
       </c>
       <c r="C146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2973,7 +2973,7 @@
         <v>1</v>
       </c>
       <c r="D147">
-        <v>100</v>
+        <v>99.99942779541016</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2981,7 +2981,7 @@
         <v>147</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D148">
         <v>100</v>
@@ -2995,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="D149">
-        <v>99.90130662918091</v>
+        <v>99.99434947967529</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3006,7 +3006,7 @@
         <v>2</v>
       </c>
       <c r="D150">
-        <v>99.99871253967285</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3017,7 +3017,7 @@
         <v>2</v>
       </c>
       <c r="D151">
-        <v>99.99958276748657</v>
+        <v>99.97072815895081</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3028,7 +3028,7 @@
         <v>2</v>
       </c>
       <c r="D152">
-        <v>99.99866485595703</v>
+        <v>99.99923706054688</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3039,7 +3039,7 @@
         <v>2</v>
       </c>
       <c r="D153">
-        <v>99.99960660934448</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3050,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="D154">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3061,7 +3061,7 @@
         <v>2</v>
       </c>
       <c r="D155">
-        <v>99.99865293502808</v>
+        <v>99.98310804367065</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3072,7 +3072,7 @@
         <v>2</v>
       </c>
       <c r="D156">
-        <v>99.9997615814209</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3083,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="D157">
-        <v>90.29697775840759</v>
+        <v>97.60161638259888</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3094,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="D158">
-        <v>99.99973773956299</v>
+        <v>100</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3105,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="D159">
-        <v>98.33279848098755</v>
+        <v>99.5122492313385</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3124,10 +3124,10 @@
         <v>160</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D161">
-        <v>99.92455244064331</v>
+        <v>100</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3138,7 +3138,7 @@
         <v>2</v>
       </c>
       <c r="D162">
-        <v>99.99488592147827</v>
+        <v>99.99979734420776</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -3146,10 +3146,10 @@
         <v>162</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D163">
-        <v>99.94003772735596</v>
+        <v>99.99887943267822</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3160,7 +3160,7 @@
         <v>2</v>
       </c>
       <c r="D164">
-        <v>98.44278693199158</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3182,7 +3182,7 @@
         <v>2</v>
       </c>
       <c r="D166">
-        <v>99.99992847442627</v>
+        <v>100</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -3215,7 +3215,7 @@
         <v>2</v>
       </c>
       <c r="D169">
-        <v>99.99970197677612</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -3259,7 +3259,7 @@
         <v>2</v>
       </c>
       <c r="D173">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3267,10 +3267,10 @@
         <v>172</v>
       </c>
       <c r="C174">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D174">
-        <v>100</v>
+        <v>99.65755343437195</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -3278,10 +3278,10 @@
         <v>172</v>
       </c>
       <c r="C175">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D175">
-        <v>100</v>
+        <v>99.65755343437195</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -3289,10 +3289,10 @@
         <v>173</v>
       </c>
       <c r="C176">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D176">
-        <v>100</v>
+        <v>99.9911904335022</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -3314,7 +3314,7 @@
         <v>2</v>
       </c>
       <c r="D178">
-        <v>99.99980926513672</v>
+        <v>100</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3325,7 +3325,7 @@
         <v>2</v>
       </c>
       <c r="D179">
-        <v>99.99939203262329</v>
+        <v>99.996018409729</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3336,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="D180">
-        <v>100</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3358,7 +3358,7 @@
         <v>2</v>
       </c>
       <c r="D182">
-        <v>99.99722242355347</v>
+        <v>99.99983310699463</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3369,7 +3369,7 @@
         <v>2</v>
       </c>
       <c r="D183">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3380,7 +3380,7 @@
         <v>2</v>
       </c>
       <c r="D184">
-        <v>93.06896924972534</v>
+        <v>100</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3388,10 +3388,10 @@
         <v>182</v>
       </c>
       <c r="C185">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D185">
-        <v>64.84900712966919</v>
+        <v>99.96150732040405</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3402,7 +3402,7 @@
         <v>2</v>
       </c>
       <c r="D186">
-        <v>99.98644590377808</v>
+        <v>100</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3410,10 +3410,10 @@
         <v>184</v>
       </c>
       <c r="C187">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D187">
-        <v>99.99977350234985</v>
+        <v>75.63840746879578</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3421,10 +3421,10 @@
         <v>185</v>
       </c>
       <c r="C188">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D188">
-        <v>99.9997615814209</v>
+        <v>99.99942779541016</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3432,10 +3432,10 @@
         <v>186</v>
       </c>
       <c r="C189">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D189">
-        <v>99.99674558639526</v>
+        <v>98.31650257110596</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3443,10 +3443,10 @@
         <v>187</v>
       </c>
       <c r="C190">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D190">
-        <v>98.83084297180176</v>
+        <v>99.7821569442749</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3479,7 +3479,7 @@
         <v>2</v>
       </c>
       <c r="D193">
-        <v>99.9966025352478</v>
+        <v>70.45386433601379</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3490,7 +3490,7 @@
         <v>2</v>
       </c>
       <c r="D194">
-        <v>99.83269572257996</v>
+        <v>57.17958211898804</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3498,10 +3498,10 @@
         <v>191</v>
       </c>
       <c r="C195">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D195">
-        <v>99.99997615814209</v>
+        <v>99.9359667301178</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3509,10 +3509,10 @@
         <v>192</v>
       </c>
       <c r="C196">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D196">
-        <v>99.99992847442627</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3523,7 +3523,7 @@
         <v>2</v>
       </c>
       <c r="D197">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>2</v>
       </c>
       <c r="D198">
-        <v>99.99988079071045</v>
+        <v>99.37750101089478</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3545,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="D199">
-        <v>99.99927282333374</v>
+        <v>100</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3567,7 +3567,7 @@
         <v>2</v>
       </c>
       <c r="D201">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3578,7 +3578,7 @@
         <v>2</v>
       </c>
       <c r="D202">
-        <v>99.78641867637634</v>
+        <v>99.99978542327881</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3600,7 +3600,7 @@
         <v>2</v>
       </c>
       <c r="D204">
-        <v>99.99902248382568</v>
+        <v>100</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3611,7 +3611,7 @@
         <v>2</v>
       </c>
       <c r="D205">
-        <v>99.9756395816803</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3622,7 +3622,7 @@
         <v>2</v>
       </c>
       <c r="D206">
-        <v>97.40889072418213</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3633,7 +3633,7 @@
         <v>2</v>
       </c>
       <c r="D207">
-        <v>99.99977350234985</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3644,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="D208">
-        <v>92.00783371925354</v>
+        <v>100</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3655,7 +3655,7 @@
         <v>2</v>
       </c>
       <c r="D209">
-        <v>78.33918929100037</v>
+        <v>99.99972581863403</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3666,7 +3666,7 @@
         <v>1</v>
       </c>
       <c r="D210">
-        <v>99.38647150993347</v>
+        <v>100</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3677,7 +3677,7 @@
         <v>2</v>
       </c>
       <c r="D211">
-        <v>90.02974629402161</v>
+        <v>100</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3688,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="D212">
-        <v>99.93599057197571</v>
+        <v>99.99936819076538</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3696,10 +3696,10 @@
         <v>209</v>
       </c>
       <c r="C213">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D213">
-        <v>60.76220273971558</v>
+        <v>92.18307137489319</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3710,7 +3710,7 @@
         <v>2</v>
       </c>
       <c r="D214">
-        <v>99.99535083770752</v>
+        <v>96.47130966186523</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3721,7 +3721,7 @@
         <v>2</v>
       </c>
       <c r="D215">
-        <v>100</v>
+        <v>99.99940395355225</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3732,7 +3732,7 @@
         <v>2</v>
       </c>
       <c r="D216">
-        <v>99.99935626983643</v>
+        <v>100</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3754,7 +3754,7 @@
         <v>2</v>
       </c>
       <c r="D218">
-        <v>99.9967098236084</v>
+        <v>100</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3765,7 +3765,7 @@
         <v>2</v>
       </c>
       <c r="D219">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3787,7 +3787,7 @@
         <v>2</v>
       </c>
       <c r="D221">
-        <v>100</v>
+        <v>99.7957706451416</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3798,7 +3798,7 @@
         <v>2</v>
       </c>
       <c r="D222">
-        <v>99.99754428863525</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3809,7 +3809,7 @@
         <v>2</v>
       </c>
       <c r="D223">
-        <v>99.99994039535522</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3820,7 +3820,7 @@
         <v>2</v>
       </c>
       <c r="D224">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3828,10 +3828,10 @@
         <v>221</v>
       </c>
       <c r="C225">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D225">
-        <v>99.9966025352478</v>
+        <v>97.36179113388062</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3853,7 +3853,7 @@
         <v>2</v>
       </c>
       <c r="D227">
-        <v>99.99998807907104</v>
+        <v>99.99892711639404</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3864,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="D228">
-        <v>99.99966621398926</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3886,7 +3886,7 @@
         <v>2</v>
       </c>
       <c r="D230">
-        <v>99.73033666610718</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3897,7 +3897,7 @@
         <v>2</v>
       </c>
       <c r="D231">
-        <v>99.99794960021973</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3905,10 +3905,10 @@
         <v>228</v>
       </c>
       <c r="C232">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D232">
-        <v>99.98828172683716</v>
+        <v>99.99964237213135</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3919,7 +3919,7 @@
         <v>1</v>
       </c>
       <c r="D233">
-        <v>97.50556945800781</v>
+        <v>99.99805688858032</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3930,7 +3930,7 @@
         <v>2</v>
       </c>
       <c r="D234">
-        <v>100</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3952,7 +3952,7 @@
         <v>1</v>
       </c>
       <c r="D236">
-        <v>99.99996423721313</v>
+        <v>100</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3963,7 +3963,7 @@
         <v>2</v>
       </c>
       <c r="D237">
-        <v>99.99990463256836</v>
+        <v>99.99797344207764</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3971,10 +3971,10 @@
         <v>234</v>
       </c>
       <c r="C238">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D238">
-        <v>99.99990463256836</v>
+        <v>99.99959468841553</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3985,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="D239">
-        <v>99.99997615814209</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -4007,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="D241">
-        <v>100</v>
+        <v>99.99984502792358</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -4018,7 +4018,7 @@
         <v>1</v>
       </c>
       <c r="D242">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -4051,7 +4051,7 @@
         <v>2</v>
       </c>
       <c r="D245">
-        <v>99.99996423721313</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -4062,7 +4062,7 @@
         <v>1</v>
       </c>
       <c r="D246">
-        <v>100</v>
+        <v>99.99988079071045</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -4081,10 +4081,10 @@
         <v>244</v>
       </c>
       <c r="C248">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D248">
-        <v>99.99983310699463</v>
+        <v>99.9994158744812</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -4095,7 +4095,7 @@
         <v>2</v>
       </c>
       <c r="D249">
-        <v>99.99997615814209</v>
+        <v>99.50218200683594</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -4106,7 +4106,7 @@
         <v>2</v>
       </c>
       <c r="D250">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -4117,7 +4117,7 @@
         <v>2</v>
       </c>
       <c r="D251">
-        <v>99.99983310699463</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -4128,7 +4128,7 @@
         <v>2</v>
       </c>
       <c r="D252">
-        <v>99.99990463256836</v>
+        <v>100</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -4136,10 +4136,10 @@
         <v>249</v>
       </c>
       <c r="C253">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D253">
-        <v>99.99918937683105</v>
+        <v>99.9671459197998</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -4161,7 +4161,7 @@
         <v>2</v>
       </c>
       <c r="D255">
-        <v>99.9997615814209</v>
+        <v>99.98916387557983</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -4172,7 +4172,7 @@
         <v>2</v>
       </c>
       <c r="D256">
-        <v>100</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4183,7 +4183,7 @@
         <v>2</v>
       </c>
       <c r="D257">
-        <v>99.99996423721313</v>
+        <v>80.00898361206055</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -4202,10 +4202,10 @@
         <v>255</v>
       </c>
       <c r="C259">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D259">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4216,7 +4216,7 @@
         <v>1</v>
       </c>
       <c r="D260">
-        <v>99.99951124191284</v>
+        <v>99.99972581863403</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -4224,10 +4224,10 @@
         <v>257</v>
       </c>
       <c r="C261">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D261">
-        <v>99.99997615814209</v>
+        <v>100</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -4246,10 +4246,10 @@
         <v>258</v>
       </c>
       <c r="C263">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D263">
-        <v>99.99998807907104</v>
+        <v>99.9914288520813</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4271,7 +4271,7 @@
         <v>2</v>
       </c>
       <c r="D265">
-        <v>99.99589920043945</v>
+        <v>100</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -4282,7 +4282,7 @@
         <v>2</v>
       </c>
       <c r="D266">
-        <v>99.96745586395264</v>
+        <v>100</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -4293,7 +4293,7 @@
         <v>2</v>
       </c>
       <c r="D267">
-        <v>99.99828338623047</v>
+        <v>99.99918937683105</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4304,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="D268">
-        <v>99.99996423721313</v>
+        <v>99.9994158744812</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4315,7 +4315,7 @@
         <v>2</v>
       </c>
       <c r="D269">
-        <v>99.99998807907104</v>
+        <v>99.99908208847046</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4323,10 +4323,10 @@
         <v>264</v>
       </c>
       <c r="C270">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D270">
-        <v>99.99992847442627</v>
+        <v>99.99984502792358</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -4337,7 +4337,7 @@
         <v>2</v>
       </c>
       <c r="D271">
-        <v>99.99997615814209</v>
+        <v>99.99908208847046</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4345,10 +4345,10 @@
         <v>266</v>
       </c>
       <c r="C272">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D272">
-        <v>74.84589219093323</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4359,7 +4359,7 @@
         <v>2</v>
       </c>
       <c r="D273">
-        <v>99.99908208847046</v>
+        <v>99.74316954612732</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4370,7 +4370,7 @@
         <v>2</v>
       </c>
       <c r="D274">
-        <v>99.99997615814209</v>
+        <v>63.5959267616272</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4378,10 +4378,10 @@
         <v>269</v>
       </c>
       <c r="C275">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D275">
-        <v>99.99972581863403</v>
+        <v>100</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4392,7 +4392,7 @@
         <v>2</v>
       </c>
       <c r="D276">
-        <v>99.99998807907104</v>
+        <v>99.98493194580078</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4403,7 +4403,7 @@
         <v>2</v>
       </c>
       <c r="D277">
-        <v>99.9998927116394</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4414,7 +4414,7 @@
         <v>2</v>
       </c>
       <c r="D278">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4425,7 +4425,7 @@
         <v>1</v>
       </c>
       <c r="D279">
-        <v>99.99980926513672</v>
+        <v>99.99992847442627</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4447,7 +4447,7 @@
         <v>2</v>
       </c>
       <c r="D281">
-        <v>99.99988079071045</v>
+        <v>99.9997615814209</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4469,7 +4469,7 @@
         <v>1</v>
       </c>
       <c r="D283">
-        <v>99.99992847442627</v>
+        <v>95.81019282341003</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4480,7 +4480,7 @@
         <v>2</v>
       </c>
       <c r="D284">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -4491,7 +4491,7 @@
         <v>2</v>
       </c>
       <c r="D285">
-        <v>99.99985694885254</v>
+        <v>100</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -4502,7 +4502,7 @@
         <v>2</v>
       </c>
       <c r="D286">
-        <v>100</v>
+        <v>99.99980926513672</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -4524,7 +4524,7 @@
         <v>2</v>
       </c>
       <c r="D288">
-        <v>99.99392032623291</v>
+        <v>99.99977350234985</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -4535,7 +4535,7 @@
         <v>2</v>
       </c>
       <c r="D289">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -4557,7 +4557,7 @@
         <v>2</v>
       </c>
       <c r="D291">
-        <v>99.99996423721313</v>
+        <v>99.99954700469971</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -4568,7 +4568,7 @@
         <v>2</v>
       </c>
       <c r="D292">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -4590,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="D294">
-        <v>99.99833106994629</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -4620,10 +4620,10 @@
         <v>290</v>
       </c>
       <c r="C297">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D297">
-        <v>100</v>
+        <v>89.43022489547729</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -4634,7 +4634,7 @@
         <v>2</v>
       </c>
       <c r="D298">
-        <v>100</v>
+        <v>99.99243021011353</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -4645,7 +4645,7 @@
         <v>2</v>
       </c>
       <c r="D299">
-        <v>100</v>
+        <v>97.71118760108948</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -4664,10 +4664,10 @@
         <v>294</v>
       </c>
       <c r="C301">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D301">
-        <v>99.99996423721313</v>
+        <v>97.75791764259338</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -4678,7 +4678,7 @@
         <v>2</v>
       </c>
       <c r="D302">
-        <v>99.99980926513672</v>
+        <v>100</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -4689,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="D303">
-        <v>99.99997615814209</v>
+        <v>99.64220523834229</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -4700,7 +4700,7 @@
         <v>2</v>
       </c>
       <c r="D304">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -4711,7 +4711,7 @@
         <v>2</v>
       </c>
       <c r="D305">
-        <v>100</v>
+        <v>99.99977350234985</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -4719,10 +4719,10 @@
         <v>299</v>
       </c>
       <c r="C306">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D306">
-        <v>50.43759346008301</v>
+        <v>99.99961853027344</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -4733,7 +4733,7 @@
         <v>2</v>
       </c>
       <c r="D307">
-        <v>99.99997615814209</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -4744,7 +4744,7 @@
         <v>2</v>
       </c>
       <c r="D308">
-        <v>99.99974966049194</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -4766,7 +4766,7 @@
         <v>2</v>
       </c>
       <c r="D310">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -4788,7 +4788,7 @@
         <v>2</v>
       </c>
       <c r="D312">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -4799,7 +4799,7 @@
         <v>2</v>
       </c>
       <c r="D313">
-        <v>99.99995231628418</v>
+        <v>99.99958276748657</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -4818,10 +4818,10 @@
         <v>307</v>
       </c>
       <c r="C315">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D315">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -4832,7 +4832,7 @@
         <v>2</v>
       </c>
       <c r="D316">
-        <v>100</v>
+        <v>99.9998927116394</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -4865,7 +4865,7 @@
         <v>2</v>
       </c>
       <c r="D319">
-        <v>99.99990463256836</v>
+        <v>99.99986886978149</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -4873,10 +4873,10 @@
         <v>312</v>
       </c>
       <c r="C320">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D320">
-        <v>100</v>
+        <v>99.78208541870117</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -4898,7 +4898,7 @@
         <v>1</v>
       </c>
       <c r="D322">
-        <v>100</v>
+        <v>99.99984502792358</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -4909,7 +4909,7 @@
         <v>1</v>
       </c>
       <c r="D323">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -4920,7 +4920,7 @@
         <v>2</v>
       </c>
       <c r="D324">
-        <v>99.99997615814209</v>
+        <v>99.99994039535522</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -4931,7 +4931,7 @@
         <v>2</v>
       </c>
       <c r="D325">
-        <v>88.48928213119507</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -4942,7 +4942,7 @@
         <v>2</v>
       </c>
       <c r="D326">
-        <v>99.99998807907104</v>
+        <v>99.99293088912964</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -4953,7 +4953,7 @@
         <v>1</v>
       </c>
       <c r="D327">
-        <v>99.99997615814209</v>
+        <v>98.95853400230408</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -4964,7 +4964,7 @@
         <v>1</v>
       </c>
       <c r="D328">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -4975,7 +4975,7 @@
         <v>1</v>
       </c>
       <c r="D329">
-        <v>99.99394416809082</v>
+        <v>99.96886253356934</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -4986,7 +4986,7 @@
         <v>1</v>
       </c>
       <c r="D330">
-        <v>99.99996423721313</v>
+        <v>100</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -4997,7 +4997,7 @@
         <v>2</v>
       </c>
       <c r="D331">
-        <v>99.99997615814209</v>
+        <v>99.99666213989258</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -5008,7 +5008,7 @@
         <v>2</v>
       </c>
       <c r="D332">
-        <v>98.47092628479004</v>
+        <v>99.95710253715515</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -5019,7 +5019,7 @@
         <v>2</v>
       </c>
       <c r="D333">
-        <v>99.99667406082153</v>
+        <v>99.99015331268311</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -5038,10 +5038,10 @@
         <v>327</v>
       </c>
       <c r="C335">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D335">
-        <v>99.99998807907104</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5060,10 +5060,10 @@
         <v>329</v>
       </c>
       <c r="C337">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D337">
-        <v>99.99921321868896</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5074,7 +5074,7 @@
         <v>2</v>
       </c>
       <c r="D338">
-        <v>99.99997615814209</v>
+        <v>99.99991655349731</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5082,10 +5082,10 @@
         <v>331</v>
       </c>
       <c r="C339">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D339">
-        <v>100</v>
+        <v>97.30446338653564</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5096,7 +5096,7 @@
         <v>1</v>
       </c>
       <c r="D340">
-        <v>100</v>
+        <v>77.00127959251404</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5104,10 +5104,10 @@
         <v>333</v>
       </c>
       <c r="C341">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D341">
-        <v>99.99991655349731</v>
+        <v>99.99978542327881</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5118,7 +5118,7 @@
         <v>1</v>
       </c>
       <c r="D342">
-        <v>100</v>
+        <v>92.62744188308716</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5126,10 +5126,10 @@
         <v>335</v>
       </c>
       <c r="C343">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D343">
-        <v>99.99997615814209</v>
+        <v>99.9970555305481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>